<commit_message>
modificados:     formularios/form_calcimp_design.py 	modificados:     formularios/form_calculo_utilidades.py 	modificados:     formularios/form_cargaremp_design.py se arreglo el ci del listado de trab que se exporta 	nuevos archivos: list_invalidados.pdf
</commit_message>
<xml_diff>
--- a/app-RRHH/file/list_opagos.xlsx
+++ b/app-RRHH/file/list_opagos.xlsx
@@ -20,7 +20,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="7">
+  <fonts count="9">
     <font>
       <name val="Calibri"/>
       <charset val="1"/>
@@ -75,6 +75,22 @@
       <b val="1"/>
       <color theme="1"/>
       <sz val="8"/>
+    </font>
+    <font>
+      <name val="CalibriCalibriCalibriCalibriCalibriCalibri"/>
+      <charset val="1"/>
+      <family val="2"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="7"/>
+    </font>
+    <font>
+      <name val="CalibriCalibriCalibriCalibriCalibriCalibriCalibri"/>
+      <charset val="1"/>
+      <family val="2"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="6"/>
     </font>
   </fonts>
   <fills count="2">
@@ -194,7 +210,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top"/>
@@ -237,6 +253,12 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -496,7 +518,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I6" sqref="I6"/>
@@ -569,24 +591,23 @@
           <t>TIPO DE PAGO</t>
         </is>
       </c>
-      <c r="G3" s="27" t="inlineStr">
+      <c r="G3" s="33" t="inlineStr">
         <is>
           <t>ABRIL</t>
         </is>
       </c>
-      <c r="H3" s="28" t="inlineStr">
+      <c r="H3" s="34" t="inlineStr">
         <is>
           <t>MAYO</t>
         </is>
       </c>
-      <c r="I3" s="29" t="inlineStr">
+      <c r="I3" s="35" t="inlineStr">
         <is>
           <t>JUNIO</t>
         </is>
       </c>
     </row>
     <row r="4"/>
-    <row r="6"/>
     <row r="1048573" ht="12.75" customHeight="1" s="9"/>
     <row r="1048574" ht="12.75" customHeight="1" s="9"/>
     <row r="1048575" ht="12.75" customHeight="1" s="9"/>

</xml_diff>

<commit_message>
nuevos archivos: file/utilidades_disteco_dpto.xlsx 	modificados:     formularios/form_calcimp_design.py terminado 	modificados:     formularios/form_calculo_utilidades.py terminado 	modificados:     formularios/form_op_design.py terminado
</commit_message>
<xml_diff>
--- a/app-RRHH/file/list_opagos.xlsx
+++ b/app-RRHH/file/list_opagos.xlsx
@@ -20,7 +20,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="9">
+  <fonts count="12">
     <font>
       <name val="Calibri"/>
       <charset val="1"/>
@@ -91,6 +91,30 @@
       <b val="1"/>
       <color theme="1"/>
       <sz val="6"/>
+    </font>
+    <font>
+      <name val="CalibriCalibriCalibriCalibriCalibriCalibriCalibriCalibri"/>
+      <charset val="1"/>
+      <family val="2"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="5"/>
+    </font>
+    <font>
+      <name val="CalibriCalibriCalibriCalibriCalibriCalibriCalibriCalibriCalibri"/>
+      <charset val="1"/>
+      <family val="2"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="4"/>
+    </font>
+    <font>
+      <name val="CalibriCalibriCalibriCalibriCalibriCalibriCalibriCalibriCalibriCalibri"/>
+      <charset val="1"/>
+      <family val="2"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -210,7 +234,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top"/>
@@ -259,6 +283,15 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -518,7 +551,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I6" sqref="I6"/>
@@ -591,23 +624,22 @@
           <t>TIPO DE PAGO</t>
         </is>
       </c>
-      <c r="G3" s="33" t="inlineStr">
+      <c r="G3" s="42" t="inlineStr">
         <is>
           <t>ABRIL</t>
         </is>
       </c>
-      <c r="H3" s="34" t="inlineStr">
+      <c r="H3" s="43" t="inlineStr">
         <is>
           <t>MAYO</t>
         </is>
       </c>
-      <c r="I3" s="35" t="inlineStr">
+      <c r="I3" s="44" t="inlineStr">
         <is>
           <t>JUNIO</t>
         </is>
       </c>
     </row>
-    <row r="4"/>
     <row r="1048573" ht="12.75" customHeight="1" s="9"/>
     <row r="1048574" ht="12.75" customHeight="1" s="9"/>
     <row r="1048575" ht="12.75" customHeight="1" s="9"/>

</xml_diff>

<commit_message>
modificados:     formularios/form_calcimp_design.py Solo queda generar dbf
</commit_message>
<xml_diff>
--- a/app-RRHH/file/list_opagos.xlsx
+++ b/app-RRHH/file/list_opagos.xlsx
@@ -20,7 +20,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <name val="Calibri"/>
       <charset val="1"/>
@@ -115,6 +115,14 @@
       <b val="1"/>
       <color theme="1"/>
       <sz val="3"/>
+    </font>
+    <font>
+      <name val="CalibriCalibriCalibriCalibriCalibriCalibriCalibriCalibriCalibriCalibriCalibri"/>
+      <charset val="1"/>
+      <family val="2"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -234,7 +242,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top"/>
@@ -292,6 +300,9 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -624,17 +635,17 @@
           <t>TIPO DE PAGO</t>
         </is>
       </c>
-      <c r="G3" s="42" t="inlineStr">
+      <c r="G3" s="45" t="inlineStr">
         <is>
           <t>ABRIL</t>
         </is>
       </c>
-      <c r="H3" s="43" t="inlineStr">
+      <c r="H3" s="46" t="inlineStr">
         <is>
           <t>MAYO</t>
         </is>
       </c>
-      <c r="I3" s="44" t="inlineStr">
+      <c r="I3" s="47" t="inlineStr">
         <is>
           <t>JUNIO</t>
         </is>

</xml_diff>